<commit_message>
Se corrigieron errores de Precedencias
</commit_message>
<xml_diff>
--- a/TablaTareasG1.xlsx
+++ b/TablaTareasG1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>Duración</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Invididual</t>
+  </si>
+  <si>
+    <t>4, 5</t>
   </si>
 </sst>
 </file>
@@ -442,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,8 +598,8 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1">
-        <v>4.5</v>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D9" s="1">
         <v>5</v>
@@ -613,7 +616,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
@@ -633,7 +636,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>

</xml_diff>